<commit_message>
:ant: Update voucher specimen metadata
</commit_message>
<xml_diff>
--- a/input_data/Molecular_data/AoW ponerine sequence source.xlsx
+++ b/input_data/Molecular_data/AoW ponerine sequence source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mael_D\R_projects\Ponerinae_Historical_Biogeography\input_data\Molecular_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Temporary Working Folder\September 2024\R_projects\Ponerinae_Historical_Biogeography\input_data\Molecular_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A265201C-0900-4A81-85D8-D99EF2508C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40E2B55-DE52-45CF-A6F6-73B8151D089E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{9F5A9187-A3CC-034C-939A-C05720182CD1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F5A9187-A3CC-034C-939A-C05720182CD1}"/>
   </bookViews>
   <sheets>
     <sheet name="phylog" sheetId="1" r:id="rId1"/>
@@ -24,23 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3468" uniqueCount="2460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3469" uniqueCount="2461">
   <si>
     <t>Current_name</t>
   </si>
@@ -7433,6 +7422,9 @@
   </si>
   <si>
     <t>This study</t>
+  </si>
+  <si>
+    <t>Camacho et al., in prep.</t>
   </si>
 </sst>
 </file>
@@ -7503,9 +7495,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7543,7 +7535,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -7649,7 +7641,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7791,7 +7783,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7802,11 +7794,11 @@
   <dimension ref="A1:K793"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G104" sqref="G104"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
@@ -21209,7 +21201,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="737" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="737" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
         <v>2101</v>
       </c>
@@ -21226,7 +21218,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="738" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="738" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
         <v>2110</v>
       </c>
@@ -21243,7 +21235,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="739" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="739" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
         <v>2119</v>
       </c>
@@ -21260,7 +21252,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="740" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="740" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
         <v>2122</v>
       </c>
@@ -21277,7 +21269,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="741" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="741" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
         <v>2125</v>
       </c>
@@ -21294,7 +21286,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="742" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="742" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
         <v>2131</v>
       </c>
@@ -21311,7 +21303,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="743" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="743" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
         <v>2140</v>
       </c>
@@ -21328,7 +21320,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="744" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="744" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
         <v>2143</v>
       </c>
@@ -21345,7 +21337,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="745" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="745" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
         <v>2146</v>
       </c>
@@ -21362,7 +21354,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="746" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="746" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
         <v>2152</v>
       </c>
@@ -21379,7 +21371,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="747" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="747" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
         <v>2155</v>
       </c>
@@ -21396,7 +21388,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="748" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="748" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
         <v>2161</v>
       </c>
@@ -21413,7 +21405,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="749" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="749" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
         <v>2164</v>
       </c>
@@ -21430,7 +21422,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="750" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="750" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
         <v>2372</v>
       </c>
@@ -21444,10 +21436,13 @@
         <v>1</v>
       </c>
       <c r="E750" t="s">
-        <v>2380</v>
-      </c>
-    </row>
-    <row r="751" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2379</v>
+      </c>
+      <c r="F750" t="s">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="751" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
         <v>2167</v>
       </c>
@@ -21464,7 +21459,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="752" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="752" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
         <v>2170</v>
       </c>

</xml_diff>